<commit_message>
Fix variable name in test configs
</commit_message>
<xml_diff>
--- a/TestComponents/TestSets/Location/FieldConfigs.xlsx
+++ b/TestComponents/TestSets/Location/FieldConfigs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepos\SVSModelBuildDeploy\TestComponents\TestSets\Location\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepos\FieldNBalance\TestComponents\TestSets\Location\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D735BE4-8617-4C3A-9CEE-8970C71219AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{783BCEF3-E583-446F-A02F-CD1480CDAD40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D0D9F3F3-C1B3-4B79-AF5D-93A117BC34BF}"/>
   </bookViews>
@@ -98,9 +98,6 @@
     <t>TestResidue05</t>
   </si>
   <si>
-    <t>PriorSaleableYield</t>
-  </si>
-  <si>
     <t>PriorFieldLoss</t>
   </si>
   <si>
@@ -143,9 +140,6 @@
     <t>CurrentCropNameFull</t>
   </si>
   <si>
-    <t>CurrentSaleableYield</t>
-  </si>
-  <si>
     <t>CurrentFieldLoss</t>
   </si>
   <si>
@@ -179,9 +173,6 @@
     <t>Oat Fodder General</t>
   </si>
   <si>
-    <t>FollowingSaleableYield</t>
-  </si>
-  <si>
     <t>FollowingFieldLoss</t>
   </si>
   <si>
@@ -285,6 +276,15 @@
   </si>
   <si>
     <t>TestResidue45</t>
+  </si>
+  <si>
+    <t>PriorFieldYield</t>
+  </si>
+  <si>
+    <t>CurrentFieldYield</t>
+  </si>
+  <si>
+    <t>FollowingFieldYield</t>
   </si>
 </sst>
 </file>
@@ -689,10 +689,10 @@
   <dimension ref="A1:N48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E29" sqref="E29"/>
+      <selection pane="bottomRight" activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,87 +703,87 @@
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" t="s">
         <v>70</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>71</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>72</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>73</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>74</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>75</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>76</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>77</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>78</v>
-      </c>
-      <c r="L1" t="s">
-        <v>79</v>
-      </c>
-      <c r="M1" t="s">
-        <v>80</v>
-      </c>
-      <c r="N1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>69</v>
-      </c>
       <c r="I2" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="M2" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="J2" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="K2" s="5" t="s">
+      <c r="N2" s="5" t="s">
         <v>66</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -1477,7 +1477,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B16" t="s">
         <v>18</v>
@@ -1533,7 +1533,7 @@
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="C17">
         <v>13</v>
@@ -1586,7 +1586,7 @@
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -1639,7 +1639,7 @@
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
       <c r="B19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -1692,7 +1692,7 @@
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C20">
         <v>13</v>
@@ -1745,7 +1745,7 @@
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C21" s="4">
         <v>44831</v>
@@ -1797,10 +1797,10 @@
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
       <c r="B22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="D22" s="3" t="str">
         <f t="shared" ref="D22:N22" si="19">C22</f>
@@ -1850,7 +1850,7 @@
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
       <c r="B23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C23" s="4">
         <v>44951</v>
@@ -1902,10 +1902,10 @@
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
       <c r="B24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="D24" s="3" t="str">
         <f t="shared" ref="D24:N24" si="21">C24</f>
@@ -1955,10 +1955,10 @@
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="9"/>
       <c r="B25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" t="s">
         <v>30</v>
-      </c>
-      <c r="C25" t="s">
-        <v>31</v>
       </c>
       <c r="D25" t="str">
         <f t="shared" ref="D25:N25" si="22">C25</f>
@@ -2008,10 +2008,10 @@
     <row r="26" spans="1:14" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="9"/>
       <c r="B26" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="D26" s="1" t="str">
         <f t="shared" ref="D26:N26" si="23">C26</f>
@@ -2060,52 +2060,52 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C27" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D27" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E27" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F27" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G27" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H27" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I27" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="J27" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="K27" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="L27" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="M27" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="N27" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28" t="s">
-        <v>35</v>
+        <v>81</v>
       </c>
       <c r="C28">
         <v>8</v>
@@ -2158,7 +2158,7 @@
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
       <c r="B29" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -2211,7 +2211,7 @@
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
       <c r="B30" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -2264,7 +2264,7 @@
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C31">
         <v>15</v>
@@ -2317,7 +2317,7 @@
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C32" s="4">
         <v>45026</v>
@@ -2369,10 +2369,10 @@
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
       <c r="B33" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D33" s="3" t="str">
         <f t="shared" ref="D33:N33" si="29">C33</f>
@@ -2422,7 +2422,7 @@
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
       <c r="B34" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C34" s="4">
         <v>45142</v>
@@ -2474,10 +2474,10 @@
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D35" s="3" t="str">
         <f t="shared" ref="D35:N35" si="31">C35</f>
@@ -2527,10 +2527,10 @@
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
       <c r="B36" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C36" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D36" t="str">
         <f t="shared" ref="D36:N36" si="32">C36</f>
@@ -2580,10 +2580,10 @@
     <row r="37" spans="1:14" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="8"/>
       <c r="B37" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D37" s="1" t="str">
         <f t="shared" ref="D37:N37" si="33">C37</f>
@@ -2632,13 +2632,13 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B38" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C38" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D38" t="str">
         <f t="shared" ref="D38:N38" si="34">C38</f>
@@ -2688,7 +2688,7 @@
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="9"/>
       <c r="B39" t="s">
-        <v>47</v>
+        <v>82</v>
       </c>
       <c r="C39">
         <v>10</v>
@@ -2741,7 +2741,7 @@
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="9"/>
       <c r="B40" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -2794,7 +2794,7 @@
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="9"/>
       <c r="B41" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -2847,7 +2847,7 @@
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="9"/>
       <c r="B42" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C42">
         <v>0</v>
@@ -2900,7 +2900,7 @@
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="9"/>
       <c r="B43" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C43" s="4">
         <v>45170</v>
@@ -2952,10 +2952,10 @@
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="9"/>
       <c r="B44" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D44" s="3" t="str">
         <f t="shared" ref="D44:N44" si="40">C44</f>
@@ -3005,7 +3005,7 @@
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="9"/>
       <c r="B45" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C45" s="4">
         <v>45200</v>
@@ -3057,10 +3057,10 @@
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="9"/>
       <c r="B46" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D46" s="3" t="str">
         <f t="shared" ref="D46:N46" si="42">C46</f>
@@ -3110,10 +3110,10 @@
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="9"/>
       <c r="B47" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C47" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D47" t="str">
         <f t="shared" ref="D47:N47" si="43">C47</f>
@@ -3163,10 +3163,10 @@
     <row r="48" spans="1:14" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="10"/>
       <c r="B48" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D48" s="1" t="str">
         <f t="shared" ref="D48:N48" si="44">C48</f>

</xml_diff>

<commit_message>
Update tests.  model was not picking up the correct soil depth value from test configs
</commit_message>
<xml_diff>
--- a/TestComponents/TestSets/Location/FieldConfigs.xlsx
+++ b/TestComponents/TestSets/Location/FieldConfigs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepos\FieldNBalance\TestComponents\TestSets\Location\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D349D4B-8D1C-41D6-90DC-22352C8837D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5DA58EF-FFA4-4D87-8CD7-2A465B89AC5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D0D9F3F3-C1B3-4B79-AF5D-93A117BC34BF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D0D9F3F3-C1B3-4B79-AF5D-93A117BC34BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="81">
   <si>
     <t>InitialN</t>
   </si>
@@ -44,9 +44,6 @@
     <t>SampleDepth</t>
   </si>
   <si>
-    <t>0-30cm</t>
-  </si>
-  <si>
     <t>PMN</t>
   </si>
   <si>
@@ -278,7 +275,10 @@
     <t>Rocks</t>
   </si>
   <si>
-    <t>Silt loam</t>
+    <t>Silt</t>
+  </si>
+  <si>
+    <t>Top30cm</t>
   </si>
 </sst>
 </file>
@@ -384,9 +384,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -424,7 +424,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -530,7 +530,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -672,7 +672,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -686,101 +686,101 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="C7" sqref="C7:N7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="27.28515625" customWidth="1"/>
-    <col min="3" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" customWidth="1"/>
+    <col min="3" max="14" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L1" t="s">
+        <v>68</v>
+      </c>
+      <c r="M1" t="s">
+        <v>69</v>
+      </c>
+      <c r="N1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G1" t="s">
-        <v>64</v>
-      </c>
-      <c r="H1" t="s">
-        <v>65</v>
-      </c>
-      <c r="I1" t="s">
-        <v>66</v>
-      </c>
-      <c r="J1" t="s">
-        <v>67</v>
-      </c>
-      <c r="K1" t="s">
-        <v>68</v>
-      </c>
-      <c r="L1" t="s">
-        <v>69</v>
-      </c>
-      <c r="M1" t="s">
-        <v>70</v>
-      </c>
-      <c r="N1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>51</v>
-      </c>
       <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="H2" s="5" t="s">
-        <v>59</v>
-      </c>
       <c r="I2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="J2" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="K2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="N2" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="N2" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="7"/>
       <c r="B3" t="s">
         <v>0</v>
@@ -833,94 +833,94 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
       <c r="B4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" t="s">
         <v>76</v>
       </c>
-      <c r="C4" t="s">
-        <v>77</v>
-      </c>
       <c r="D4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="7"/>
       <c r="B6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -959,2059 +959,2048 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="8"/>
       <c r="B7" t="s">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" t="str">
-        <f t="shared" ref="D7:N7" si="1">C7</f>
-        <v>0-30cm</v>
-      </c>
-      <c r="E7" t="str">
-        <f t="shared" si="1"/>
-        <v>0-30cm</v>
-      </c>
-      <c r="F7" t="str">
-        <f t="shared" si="1"/>
-        <v>0-30cm</v>
-      </c>
-      <c r="G7" t="str">
-        <f t="shared" si="1"/>
-        <v>0-30cm</v>
-      </c>
-      <c r="H7" t="str">
-        <f t="shared" si="1"/>
-        <v>0-30cm</v>
-      </c>
-      <c r="I7" t="str">
-        <f t="shared" si="1"/>
-        <v>0-30cm</v>
-      </c>
-      <c r="J7" t="str">
-        <f t="shared" si="1"/>
-        <v>0-30cm</v>
-      </c>
-      <c r="K7" t="str">
-        <f t="shared" si="1"/>
-        <v>0-30cm</v>
-      </c>
-      <c r="L7" t="str">
-        <f t="shared" si="1"/>
-        <v>0-30cm</v>
-      </c>
-      <c r="M7" t="str">
-        <f t="shared" si="1"/>
-        <v>0-30cm</v>
-      </c>
-      <c r="N7" t="str">
-        <f t="shared" si="1"/>
-        <v>0-30cm</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="D7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E7" t="s">
+        <v>80</v>
+      </c>
+      <c r="F7" t="s">
+        <v>80</v>
+      </c>
+      <c r="G7" t="s">
+        <v>80</v>
+      </c>
+      <c r="H7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I7" t="s">
+        <v>80</v>
+      </c>
+      <c r="J7" t="s">
+        <v>80</v>
+      </c>
+      <c r="K7" t="s">
+        <v>80</v>
+      </c>
+      <c r="L7" t="s">
+        <v>80</v>
+      </c>
+      <c r="M7" t="s">
+        <v>80</v>
+      </c>
+      <c r="N7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="8"/>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8">
         <v>50</v>
       </c>
       <c r="D8">
-        <f t="shared" ref="D8:N8" si="2">C8</f>
+        <f t="shared" ref="D8:N8" si="1">C8</f>
         <v>50</v>
       </c>
       <c r="E8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="F8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="G8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="H8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="I8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="J8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="K8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="L8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="M8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="N8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="8"/>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C9">
         <v>3</v>
       </c>
       <c r="D9">
-        <f t="shared" ref="D9:N9" si="3">C9</f>
+        <f t="shared" ref="D9:N9" si="2">C9</f>
         <v>3</v>
       </c>
       <c r="E9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="F9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="G9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="H9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="I9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="J9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="K9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="L9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="M9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="N9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="8"/>
       <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
         <v>5</v>
       </c>
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
       <c r="D10" t="str">
-        <f t="shared" ref="D10:N10" si="4">C10</f>
+        <f t="shared" ref="D10:N10" si="3">C10</f>
         <v>Typical</v>
       </c>
       <c r="E10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>Typical</v>
       </c>
       <c r="F10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>Typical</v>
       </c>
       <c r="G10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>Typical</v>
       </c>
       <c r="H10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>Typical</v>
       </c>
       <c r="I10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>Typical</v>
       </c>
       <c r="J10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>Typical</v>
       </c>
       <c r="K10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>Typical</v>
       </c>
       <c r="L10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>Typical</v>
       </c>
       <c r="M10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>Typical</v>
       </c>
       <c r="N10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>Typical</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="8"/>
       <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
         <v>7</v>
       </c>
-      <c r="C11" t="s">
-        <v>8</v>
-      </c>
       <c r="D11" t="str">
-        <f t="shared" ref="D11:N11" si="5">C11</f>
+        <f t="shared" ref="D11:N11" si="4">C11</f>
         <v>Very Dry</v>
       </c>
       <c r="E11" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Very Dry</v>
       </c>
       <c r="F11" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Very Dry</v>
       </c>
       <c r="G11" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Very Dry</v>
       </c>
       <c r="H11" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Very Dry</v>
       </c>
       <c r="I11" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Very Dry</v>
       </c>
       <c r="J11" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Very Dry</v>
       </c>
       <c r="K11" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Very Dry</v>
       </c>
       <c r="L11" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Very Dry</v>
       </c>
       <c r="M11" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Very Dry</v>
       </c>
       <c r="N11" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Very Dry</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="8"/>
       <c r="B12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="str">
+        <f t="shared" ref="D12:N12" si="5">C12</f>
+        <v>Full</v>
+      </c>
+      <c r="E12" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>Full</v>
+      </c>
+      <c r="F12" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>Full</v>
+      </c>
+      <c r="G12" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>Full</v>
+      </c>
+      <c r="H12" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>Full</v>
+      </c>
+      <c r="I12" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>Full</v>
+      </c>
+      <c r="J12" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>Full</v>
+      </c>
+      <c r="K12" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>Full</v>
+      </c>
+      <c r="L12" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>Full</v>
+      </c>
+      <c r="M12" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>Full</v>
+      </c>
+      <c r="N12" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>Full</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="1" t="str">
-        <f t="shared" ref="D12:N12" si="6">C12</f>
-        <v>Full</v>
-      </c>
-      <c r="E12" s="1" t="str">
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" ref="D13:N13" si="6">C13</f>
+        <v>TestResidue05</v>
+      </c>
+      <c r="E13" t="str">
         <f t="shared" si="6"/>
-        <v>Full</v>
-      </c>
-      <c r="F12" s="1" t="str">
+        <v>TestResidue05</v>
+      </c>
+      <c r="F13" t="str">
         <f t="shared" si="6"/>
-        <v>Full</v>
-      </c>
-      <c r="G12" s="1" t="str">
+        <v>TestResidue05</v>
+      </c>
+      <c r="G13" t="str">
         <f t="shared" si="6"/>
-        <v>Full</v>
-      </c>
-      <c r="H12" s="1" t="str">
+        <v>TestResidue05</v>
+      </c>
+      <c r="H13" t="str">
         <f t="shared" si="6"/>
-        <v>Full</v>
-      </c>
-      <c r="I12" s="1" t="str">
+        <v>TestResidue05</v>
+      </c>
+      <c r="I13" t="str">
         <f t="shared" si="6"/>
-        <v>Full</v>
-      </c>
-      <c r="J12" s="1" t="str">
+        <v>TestResidue05</v>
+      </c>
+      <c r="J13" t="str">
         <f t="shared" si="6"/>
-        <v>Full</v>
-      </c>
-      <c r="K12" s="1" t="str">
+        <v>TestResidue05</v>
+      </c>
+      <c r="K13" t="str">
         <f t="shared" si="6"/>
-        <v>Full</v>
-      </c>
-      <c r="L12" s="1" t="str">
+        <v>TestResidue05</v>
+      </c>
+      <c r="L13" t="str">
         <f t="shared" si="6"/>
-        <v>Full</v>
-      </c>
-      <c r="M12" s="1" t="str">
+        <v>TestResidue05</v>
+      </c>
+      <c r="M13" t="str">
         <f t="shared" si="6"/>
-        <v>Full</v>
-      </c>
-      <c r="N12" s="1" t="str">
+        <v>TestResidue05</v>
+      </c>
+      <c r="N13" t="str">
         <f t="shared" si="6"/>
-        <v>Full</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" t="str">
-        <f t="shared" ref="D13:N13" si="7">C13</f>
         <v>TestResidue05</v>
       </c>
-      <c r="E13" t="str">
-        <f t="shared" si="7"/>
-        <v>TestResidue05</v>
-      </c>
-      <c r="F13" t="str">
-        <f t="shared" si="7"/>
-        <v>TestResidue05</v>
-      </c>
-      <c r="G13" t="str">
-        <f t="shared" si="7"/>
-        <v>TestResidue05</v>
-      </c>
-      <c r="H13" t="str">
-        <f t="shared" si="7"/>
-        <v>TestResidue05</v>
-      </c>
-      <c r="I13" t="str">
-        <f t="shared" si="7"/>
-        <v>TestResidue05</v>
-      </c>
-      <c r="J13" t="str">
-        <f t="shared" si="7"/>
-        <v>TestResidue05</v>
-      </c>
-      <c r="K13" t="str">
-        <f t="shared" si="7"/>
-        <v>TestResidue05</v>
-      </c>
-      <c r="L13" t="str">
-        <f t="shared" si="7"/>
-        <v>TestResidue05</v>
-      </c>
-      <c r="M13" t="str">
-        <f t="shared" si="7"/>
-        <v>TestResidue05</v>
-      </c>
-      <c r="N13" t="str">
-        <f t="shared" si="7"/>
-        <v>TestResidue05</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="9"/>
       <c r="B14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C14">
         <v>13</v>
       </c>
       <c r="D14">
-        <f t="shared" ref="D14:N14" si="8">C14</f>
+        <f t="shared" ref="D14:N14" si="7">C14</f>
         <v>13</v>
       </c>
       <c r="E14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>13</v>
       </c>
       <c r="F14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>13</v>
       </c>
       <c r="G14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>13</v>
       </c>
       <c r="H14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>13</v>
       </c>
       <c r="I14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>13</v>
       </c>
       <c r="J14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>13</v>
       </c>
       <c r="K14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>13</v>
       </c>
       <c r="L14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>13</v>
       </c>
       <c r="M14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>13</v>
       </c>
       <c r="N14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="9"/>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15">
-        <f t="shared" ref="D15:N15" si="9">C15</f>
+        <f t="shared" ref="D15:N15" si="8">C15</f>
         <v>0</v>
       </c>
       <c r="E15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="H15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="L15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="M15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="N15">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="9"/>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="D16">
-        <f t="shared" ref="D16:N16" si="10">C16</f>
+        <f t="shared" ref="D16:N16" si="9">C16</f>
         <v>0</v>
       </c>
       <c r="E16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="G16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="I16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="K16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="L16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="M16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N16">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="9"/>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17">
         <v>13</v>
       </c>
       <c r="D17">
-        <f t="shared" ref="D17:N17" si="11">C17</f>
+        <f t="shared" ref="D17:N17" si="10">C17</f>
         <v>13</v>
       </c>
       <c r="E17">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>13</v>
       </c>
       <c r="F17">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>13</v>
       </c>
       <c r="G17">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>13</v>
       </c>
       <c r="H17">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>13</v>
       </c>
       <c r="I17">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>13</v>
       </c>
       <c r="J17">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>13</v>
       </c>
       <c r="K17">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>13</v>
       </c>
       <c r="L17">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>13</v>
       </c>
       <c r="M17">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>13</v>
       </c>
       <c r="N17">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="9"/>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C18" s="4">
         <v>44831</v>
       </c>
       <c r="D18" s="4">
-        <f t="shared" ref="D18:N18" si="12">C18</f>
+        <f t="shared" ref="D18:N18" si="11">C18</f>
         <v>44831</v>
       </c>
       <c r="E18" s="4">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>44831</v>
       </c>
       <c r="F18" s="4">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>44831</v>
       </c>
       <c r="G18" s="4">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>44831</v>
       </c>
       <c r="H18" s="4">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>44831</v>
       </c>
       <c r="I18" s="6">
         <v>45026</v>
       </c>
       <c r="J18" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>45026</v>
       </c>
       <c r="K18" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>45026</v>
       </c>
       <c r="L18" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>45026</v>
       </c>
       <c r="M18" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>45026</v>
       </c>
       <c r="N18" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>45026</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="9"/>
       <c r="B19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="D19" s="3" t="str">
-        <f t="shared" ref="D19:N19" si="13">C19</f>
+        <f t="shared" ref="D19:N19" si="12">C19</f>
         <v>Seed</v>
       </c>
       <c r="E19" s="3" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>Seed</v>
       </c>
       <c r="F19" s="3" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>Seed</v>
       </c>
       <c r="G19" s="3" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>Seed</v>
       </c>
       <c r="H19" s="3" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>Seed</v>
       </c>
       <c r="I19" s="3" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>Seed</v>
       </c>
       <c r="J19" s="3" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>Seed</v>
       </c>
       <c r="K19" s="3" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>Seed</v>
       </c>
       <c r="L19" s="3" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>Seed</v>
       </c>
       <c r="M19" s="3" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>Seed</v>
       </c>
       <c r="N19" s="3" t="str">
-        <f t="shared" si="13"/>
-        <v>Seed</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="12"/>
+        <v>Seed</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="9"/>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C20" s="4">
         <v>44951</v>
       </c>
       <c r="D20" s="4">
-        <f t="shared" ref="D20:N20" si="14">C20</f>
+        <f t="shared" ref="D20:N20" si="13">C20</f>
         <v>44951</v>
       </c>
       <c r="E20" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>44951</v>
       </c>
       <c r="F20" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>44951</v>
       </c>
       <c r="G20" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>44951</v>
       </c>
       <c r="H20" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>44951</v>
       </c>
       <c r="I20" s="6">
         <v>45142</v>
       </c>
       <c r="J20" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>45142</v>
       </c>
       <c r="K20" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>45142</v>
       </c>
       <c r="L20" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>45142</v>
       </c>
       <c r="M20" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>45142</v>
       </c>
       <c r="N20" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>45142</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="9"/>
       <c r="B21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="D21" s="3" t="str">
-        <f t="shared" ref="D21:N21" si="15">C21</f>
+        <f t="shared" ref="D21:N21" si="14">C21</f>
         <v>Maturity</v>
       </c>
       <c r="E21" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>Maturity</v>
       </c>
       <c r="F21" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>Maturity</v>
       </c>
       <c r="G21" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>Maturity</v>
       </c>
       <c r="H21" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>Maturity</v>
       </c>
       <c r="I21" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>Maturity</v>
       </c>
       <c r="J21" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>Maturity</v>
       </c>
       <c r="K21" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>Maturity</v>
       </c>
       <c r="L21" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>Maturity</v>
       </c>
       <c r="M21" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>Maturity</v>
       </c>
       <c r="N21" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>Maturity</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="9"/>
       <c r="B22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" t="s">
         <v>22</v>
       </c>
-      <c r="C22" t="s">
-        <v>23</v>
-      </c>
       <c r="D22" t="str">
-        <f t="shared" ref="D22:N22" si="16">C22</f>
+        <f t="shared" ref="D22:N22" si="15">C22</f>
         <v>None removed</v>
       </c>
       <c r="E22" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>None removed</v>
       </c>
       <c r="F22" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>None removed</v>
       </c>
       <c r="G22" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>None removed</v>
       </c>
       <c r="H22" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>None removed</v>
       </c>
       <c r="I22" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>None removed</v>
       </c>
       <c r="J22" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>None removed</v>
       </c>
       <c r="K22" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>None removed</v>
       </c>
       <c r="L22" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>None removed</v>
       </c>
       <c r="M22" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>None removed</v>
       </c>
       <c r="N22" t="str">
-        <f t="shared" si="16"/>
-        <v>None removed</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="15"/>
+        <v>None removed</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="9"/>
       <c r="B23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="D23" s="1" t="str">
+        <f t="shared" ref="D23:N23" si="16">C23</f>
+        <v>Full (Plough)</v>
+      </c>
+      <c r="E23" s="1" t="str">
+        <f t="shared" si="16"/>
+        <v>Full (Plough)</v>
+      </c>
+      <c r="F23" s="1" t="str">
+        <f t="shared" si="16"/>
+        <v>Full (Plough)</v>
+      </c>
+      <c r="G23" s="1" t="str">
+        <f t="shared" si="16"/>
+        <v>Full (Plough)</v>
+      </c>
+      <c r="H23" s="1" t="str">
+        <f t="shared" si="16"/>
+        <v>Full (Plough)</v>
+      </c>
+      <c r="I23" s="1" t="str">
+        <f t="shared" si="16"/>
+        <v>Full (Plough)</v>
+      </c>
+      <c r="J23" s="1" t="str">
+        <f t="shared" si="16"/>
+        <v>Full (Plough)</v>
+      </c>
+      <c r="K23" s="1" t="str">
+        <f t="shared" si="16"/>
+        <v>Full (Plough)</v>
+      </c>
+      <c r="L23" s="1" t="str">
+        <f t="shared" si="16"/>
+        <v>Full (Plough)</v>
+      </c>
+      <c r="M23" s="1" t="str">
+        <f t="shared" si="16"/>
+        <v>Full (Plough)</v>
+      </c>
+      <c r="N23" s="1" t="str">
+        <f t="shared" si="16"/>
+        <v>Full (Plough)</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A24" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" t="s">
         <v>25</v>
       </c>
-      <c r="D23" s="1" t="str">
-        <f t="shared" ref="D23:N23" si="17">C23</f>
-        <v>Full (Plough)</v>
-      </c>
-      <c r="E23" s="1" t="str">
-        <f t="shared" si="17"/>
-        <v>Full (Plough)</v>
-      </c>
-      <c r="F23" s="1" t="str">
-        <f t="shared" si="17"/>
-        <v>Full (Plough)</v>
-      </c>
-      <c r="G23" s="1" t="str">
-        <f t="shared" si="17"/>
-        <v>Full (Plough)</v>
-      </c>
-      <c r="H23" s="1" t="str">
-        <f t="shared" si="17"/>
-        <v>Full (Plough)</v>
-      </c>
-      <c r="I23" s="1" t="str">
-        <f t="shared" si="17"/>
-        <v>Full (Plough)</v>
-      </c>
-      <c r="J23" s="1" t="str">
-        <f t="shared" si="17"/>
-        <v>Full (Plough)</v>
-      </c>
-      <c r="K23" s="1" t="str">
-        <f t="shared" si="17"/>
-        <v>Full (Plough)</v>
-      </c>
-      <c r="L23" s="1" t="str">
-        <f t="shared" si="17"/>
-        <v>Full (Plough)</v>
-      </c>
-      <c r="M23" s="1" t="str">
-        <f t="shared" si="17"/>
-        <v>Full (Plough)</v>
-      </c>
-      <c r="N23" s="1" t="str">
-        <f t="shared" si="17"/>
-        <v>Full (Plough)</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B24" t="s">
-        <v>26</v>
-      </c>
       <c r="C24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N24" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="8"/>
       <c r="B25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C25">
         <v>8</v>
       </c>
       <c r="D25">
-        <f t="shared" ref="D25:N25" si="18">C25</f>
+        <f t="shared" ref="D25:N25" si="17">C25</f>
         <v>8</v>
       </c>
       <c r="E25">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>8</v>
       </c>
       <c r="F25">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>8</v>
       </c>
       <c r="G25">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>8</v>
       </c>
       <c r="H25">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>8</v>
       </c>
       <c r="I25">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>8</v>
       </c>
       <c r="J25">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>8</v>
       </c>
       <c r="K25">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>8</v>
       </c>
       <c r="L25">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>8</v>
       </c>
       <c r="M25">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>8</v>
       </c>
       <c r="N25">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="8"/>
       <c r="B26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C26">
         <v>0</v>
       </c>
       <c r="D26">
-        <f t="shared" ref="D26:N26" si="19">C26</f>
+        <f t="shared" ref="D26:N26" si="18">C26</f>
         <v>0</v>
       </c>
       <c r="E26">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="F26">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="G26">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H26">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="I26">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="J26">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="K26">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="L26">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="M26">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="N26">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" s="8"/>
       <c r="B27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C27">
         <v>0</v>
       </c>
       <c r="D27">
-        <f t="shared" ref="D27:N27" si="20">C27</f>
+        <f t="shared" ref="D27:N27" si="19">C27</f>
         <v>0</v>
       </c>
       <c r="E27">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="F27">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="G27">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="H27">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="I27">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="J27">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="K27">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="L27">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="M27">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="N27">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" s="8"/>
       <c r="B28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C28">
         <v>15</v>
       </c>
       <c r="D28">
-        <f t="shared" ref="D28:N28" si="21">C28</f>
+        <f t="shared" ref="D28:N28" si="20">C28</f>
         <v>15</v>
       </c>
       <c r="E28">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>15</v>
       </c>
       <c r="F28">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>15</v>
       </c>
       <c r="G28">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>15</v>
       </c>
       <c r="H28">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>15</v>
       </c>
       <c r="I28">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>15</v>
       </c>
       <c r="J28">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>15</v>
       </c>
       <c r="K28">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>15</v>
       </c>
       <c r="L28">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>15</v>
       </c>
       <c r="M28">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>15</v>
       </c>
       <c r="N28">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="8"/>
       <c r="B29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C29" s="4">
         <v>45026</v>
       </c>
       <c r="D29" s="4">
-        <f t="shared" ref="D29:N29" si="22">C29</f>
+        <f t="shared" ref="D29:N29" si="21">C29</f>
         <v>45026</v>
       </c>
       <c r="E29" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>45026</v>
       </c>
       <c r="F29" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>45026</v>
       </c>
       <c r="G29" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>45026</v>
       </c>
       <c r="H29" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>45026</v>
       </c>
       <c r="I29" s="6">
         <v>45170</v>
       </c>
       <c r="J29" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>45170</v>
       </c>
       <c r="K29" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>45170</v>
       </c>
       <c r="L29" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>45170</v>
       </c>
       <c r="M29" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>45170</v>
       </c>
       <c r="N29" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>45170</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" s="8"/>
       <c r="B30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D30" s="3" t="str">
-        <f t="shared" ref="D30:N30" si="23">C30</f>
+        <f t="shared" ref="D30:N30" si="22">C30</f>
         <v>Seed</v>
       </c>
       <c r="E30" s="3" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>Seed</v>
       </c>
       <c r="F30" s="3" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>Seed</v>
       </c>
       <c r="G30" s="3" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>Seed</v>
       </c>
       <c r="H30" s="3" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>Seed</v>
       </c>
       <c r="I30" s="3" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>Seed</v>
       </c>
       <c r="J30" s="3" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>Seed</v>
       </c>
       <c r="K30" s="3" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>Seed</v>
       </c>
       <c r="L30" s="3" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>Seed</v>
       </c>
       <c r="M30" s="3" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>Seed</v>
       </c>
       <c r="N30" s="3" t="str">
-        <f t="shared" si="23"/>
-        <v>Seed</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="22"/>
+        <v>Seed</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" s="8"/>
       <c r="B31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C31" s="4">
         <v>45142</v>
       </c>
       <c r="D31" s="4">
-        <f t="shared" ref="D31:N31" si="24">C31</f>
+        <f t="shared" ref="D31:N31" si="23">C31</f>
         <v>45142</v>
       </c>
       <c r="E31" s="4">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>45142</v>
       </c>
       <c r="F31" s="4">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>45142</v>
       </c>
       <c r="G31" s="4">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>45142</v>
       </c>
       <c r="H31" s="4">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>45142</v>
       </c>
       <c r="I31" s="6">
         <v>45261</v>
       </c>
       <c r="J31" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>45261</v>
       </c>
       <c r="K31" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>45261</v>
       </c>
       <c r="L31" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>45261</v>
       </c>
       <c r="M31" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>45261</v>
       </c>
       <c r="N31" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>45261</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="8"/>
       <c r="B32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D32" s="3" t="str">
-        <f t="shared" ref="D32:N32" si="25">C32</f>
+        <f t="shared" ref="D32:N32" si="24">C32</f>
         <v>Maturity</v>
       </c>
       <c r="E32" s="3" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>Maturity</v>
       </c>
       <c r="F32" s="3" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>Maturity</v>
       </c>
       <c r="G32" s="3" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>Maturity</v>
       </c>
       <c r="H32" s="3" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>Maturity</v>
       </c>
       <c r="I32" s="3" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>Maturity</v>
       </c>
       <c r="J32" s="3" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>Maturity</v>
       </c>
       <c r="K32" s="3" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>Maturity</v>
       </c>
       <c r="L32" s="3" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>Maturity</v>
       </c>
       <c r="M32" s="3" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>Maturity</v>
       </c>
       <c r="N32" s="3" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>Maturity</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" s="8"/>
       <c r="B33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C33" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D33" t="str">
-        <f t="shared" ref="D33:N33" si="26">C33</f>
+        <f t="shared" ref="D33:N33" si="25">C33</f>
         <v>None removed</v>
       </c>
       <c r="E33" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>None removed</v>
       </c>
       <c r="F33" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>None removed</v>
       </c>
       <c r="G33" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>None removed</v>
       </c>
       <c r="H33" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>None removed</v>
       </c>
       <c r="I33" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>None removed</v>
       </c>
       <c r="J33" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>None removed</v>
       </c>
       <c r="K33" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>None removed</v>
       </c>
       <c r="L33" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>None removed</v>
       </c>
       <c r="M33" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>None removed</v>
       </c>
       <c r="N33" t="str">
-        <f t="shared" si="26"/>
-        <v>None removed</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="25"/>
+        <v>None removed</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="8"/>
       <c r="B34" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D34" s="1" t="str">
+        <f t="shared" ref="D34:N34" si="26">C34</f>
+        <v>Full (Plough)</v>
+      </c>
+      <c r="E34" s="1" t="str">
+        <f t="shared" si="26"/>
+        <v>Full (Plough)</v>
+      </c>
+      <c r="F34" s="1" t="str">
+        <f t="shared" si="26"/>
+        <v>Full (Plough)</v>
+      </c>
+      <c r="G34" s="1" t="str">
+        <f t="shared" si="26"/>
+        <v>Full (Plough)</v>
+      </c>
+      <c r="H34" s="1" t="str">
+        <f t="shared" si="26"/>
+        <v>Full (Plough)</v>
+      </c>
+      <c r="I34" s="1" t="str">
+        <f t="shared" si="26"/>
+        <v>Full (Plough)</v>
+      </c>
+      <c r="J34" s="1" t="str">
+        <f t="shared" si="26"/>
+        <v>Full (Plough)</v>
+      </c>
+      <c r="K34" s="1" t="str">
+        <f t="shared" si="26"/>
+        <v>Full (Plough)</v>
+      </c>
+      <c r="L34" s="1" t="str">
+        <f t="shared" si="26"/>
+        <v>Full (Plough)</v>
+      </c>
+      <c r="M34" s="1" t="str">
+        <f t="shared" si="26"/>
+        <v>Full (Plough)</v>
+      </c>
+      <c r="N34" s="1" t="str">
+        <f t="shared" si="26"/>
+        <v>Full (Plough)</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A35" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B35" t="s">
         <v>35</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D34" s="1" t="str">
-        <f t="shared" ref="D34:N34" si="27">C34</f>
-        <v>Full (Plough)</v>
-      </c>
-      <c r="E34" s="1" t="str">
+      <c r="C35" t="s">
+        <v>36</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" ref="D35:N35" si="27">C35</f>
+        <v>Oat Fodder General</v>
+      </c>
+      <c r="E35" t="str">
         <f t="shared" si="27"/>
-        <v>Full (Plough)</v>
-      </c>
-      <c r="F34" s="1" t="str">
+        <v>Oat Fodder General</v>
+      </c>
+      <c r="F35" t="str">
         <f t="shared" si="27"/>
-        <v>Full (Plough)</v>
-      </c>
-      <c r="G34" s="1" t="str">
+        <v>Oat Fodder General</v>
+      </c>
+      <c r="G35" t="str">
         <f t="shared" si="27"/>
-        <v>Full (Plough)</v>
-      </c>
-      <c r="H34" s="1" t="str">
+        <v>Oat Fodder General</v>
+      </c>
+      <c r="H35" t="str">
         <f t="shared" si="27"/>
-        <v>Full (Plough)</v>
-      </c>
-      <c r="I34" s="1" t="str">
+        <v>Oat Fodder General</v>
+      </c>
+      <c r="I35" t="str">
         <f t="shared" si="27"/>
-        <v>Full (Plough)</v>
-      </c>
-      <c r="J34" s="1" t="str">
+        <v>Oat Fodder General</v>
+      </c>
+      <c r="J35" t="str">
         <f t="shared" si="27"/>
-        <v>Full (Plough)</v>
-      </c>
-      <c r="K34" s="1" t="str">
+        <v>Oat Fodder General</v>
+      </c>
+      <c r="K35" t="str">
         <f t="shared" si="27"/>
-        <v>Full (Plough)</v>
-      </c>
-      <c r="L34" s="1" t="str">
+        <v>Oat Fodder General</v>
+      </c>
+      <c r="L35" t="str">
         <f t="shared" si="27"/>
-        <v>Full (Plough)</v>
-      </c>
-      <c r="M34" s="1" t="str">
+        <v>Oat Fodder General</v>
+      </c>
+      <c r="M35" t="str">
         <f t="shared" si="27"/>
-        <v>Full (Plough)</v>
-      </c>
-      <c r="N34" s="1" t="str">
+        <v>Oat Fodder General</v>
+      </c>
+      <c r="N35" t="str">
         <f t="shared" si="27"/>
-        <v>Full (Plough)</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="B35" t="s">
-        <v>36</v>
-      </c>
-      <c r="C35" t="s">
-        <v>37</v>
-      </c>
-      <c r="D35" t="str">
-        <f t="shared" ref="D35:N35" si="28">C35</f>
         <v>Oat Fodder General</v>
       </c>
-      <c r="E35" t="str">
-        <f t="shared" si="28"/>
-        <v>Oat Fodder General</v>
-      </c>
-      <c r="F35" t="str">
-        <f t="shared" si="28"/>
-        <v>Oat Fodder General</v>
-      </c>
-      <c r="G35" t="str">
-        <f t="shared" si="28"/>
-        <v>Oat Fodder General</v>
-      </c>
-      <c r="H35" t="str">
-        <f t="shared" si="28"/>
-        <v>Oat Fodder General</v>
-      </c>
-      <c r="I35" t="str">
-        <f t="shared" si="28"/>
-        <v>Oat Fodder General</v>
-      </c>
-      <c r="J35" t="str">
-        <f t="shared" si="28"/>
-        <v>Oat Fodder General</v>
-      </c>
-      <c r="K35" t="str">
-        <f t="shared" si="28"/>
-        <v>Oat Fodder General</v>
-      </c>
-      <c r="L35" t="str">
-        <f t="shared" si="28"/>
-        <v>Oat Fodder General</v>
-      </c>
-      <c r="M35" t="str">
-        <f t="shared" si="28"/>
-        <v>Oat Fodder General</v>
-      </c>
-      <c r="N35" t="str">
-        <f t="shared" si="28"/>
-        <v>Oat Fodder General</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" s="9"/>
       <c r="B36" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C36">
         <v>10</v>
       </c>
       <c r="D36">
-        <f t="shared" ref="D36:N36" si="29">C36</f>
+        <f t="shared" ref="D36:N36" si="28">C36</f>
         <v>10</v>
       </c>
       <c r="E36">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>10</v>
       </c>
       <c r="F36">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>10</v>
       </c>
       <c r="G36">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>10</v>
       </c>
       <c r="H36">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>10</v>
       </c>
       <c r="I36">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>10</v>
       </c>
       <c r="J36">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>10</v>
       </c>
       <c r="K36">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>10</v>
       </c>
       <c r="L36">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>10</v>
       </c>
       <c r="M36">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>10</v>
       </c>
       <c r="N36">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" s="9"/>
       <c r="B37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C37">
         <v>0</v>
       </c>
       <c r="D37">
-        <f t="shared" ref="D37:N37" si="30">C37</f>
+        <f t="shared" ref="D37:N37" si="29">C37</f>
         <v>0</v>
       </c>
       <c r="E37">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="F37">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="G37">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="H37">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="I37">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="J37">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="K37">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="L37">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="M37">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="N37">
-        <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" s="9"/>
       <c r="B38" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C38">
         <v>0</v>
       </c>
       <c r="D38">
-        <f t="shared" ref="D38:N38" si="31">C38</f>
+        <f t="shared" ref="D38:N38" si="30">C38</f>
         <v>0</v>
       </c>
       <c r="E38">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="F38">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="G38">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="H38">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="I38">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="J38">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="K38">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="L38">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="M38">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="N38">
-        <f t="shared" si="31"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" s="9"/>
       <c r="B39" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C39">
         <v>0</v>
       </c>
       <c r="D39">
-        <f t="shared" ref="D39:N39" si="32">C39</f>
+        <f t="shared" ref="D39:N39" si="31">C39</f>
         <v>0</v>
       </c>
       <c r="E39">
-        <f t="shared" si="32"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="F39">
-        <f t="shared" si="32"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="G39">
-        <f t="shared" si="32"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="H39">
-        <f t="shared" si="32"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="I39">
-        <f t="shared" si="32"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="J39">
-        <f t="shared" si="32"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="K39">
-        <f t="shared" si="32"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="L39">
-        <f t="shared" si="32"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="M39">
-        <f t="shared" si="32"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="N39">
-        <f t="shared" si="32"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" s="9"/>
       <c r="B40" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C40" s="4">
         <v>45170</v>
       </c>
       <c r="D40" s="4">
-        <f t="shared" ref="D40:N40" si="33">C40</f>
+        <f t="shared" ref="D40:N40" si="32">C40</f>
         <v>45170</v>
       </c>
       <c r="E40" s="4">
-        <f t="shared" si="33"/>
+        <f t="shared" si="32"/>
         <v>45170</v>
       </c>
       <c r="F40" s="4">
-        <f t="shared" si="33"/>
+        <f t="shared" si="32"/>
         <v>45170</v>
       </c>
       <c r="G40" s="4">
-        <f t="shared" si="33"/>
+        <f t="shared" si="32"/>
         <v>45170</v>
       </c>
       <c r="H40" s="4">
-        <f t="shared" si="33"/>
+        <f t="shared" si="32"/>
         <v>45170</v>
       </c>
       <c r="I40" s="6">
         <v>45292</v>
       </c>
       <c r="J40" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="32"/>
         <v>45292</v>
       </c>
       <c r="K40" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="32"/>
         <v>45292</v>
       </c>
       <c r="L40" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="32"/>
         <v>45292</v>
       </c>
       <c r="M40" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="32"/>
         <v>45292</v>
       </c>
       <c r="N40" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="32"/>
         <v>45292</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" s="9"/>
       <c r="B41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D41" s="3" t="str">
-        <f t="shared" ref="D41:N41" si="34">C41</f>
+        <f t="shared" ref="D41:N41" si="33">C41</f>
         <v>Seed</v>
       </c>
       <c r="E41" s="3" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="33"/>
         <v>Seed</v>
       </c>
       <c r="F41" s="3" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="33"/>
         <v>Seed</v>
       </c>
       <c r="G41" s="3" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="33"/>
         <v>Seed</v>
       </c>
       <c r="H41" s="3" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="33"/>
         <v>Seed</v>
       </c>
       <c r="I41" s="3" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="33"/>
         <v>Seed</v>
       </c>
       <c r="J41" s="3" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="33"/>
         <v>Seed</v>
       </c>
       <c r="K41" s="3" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="33"/>
         <v>Seed</v>
       </c>
       <c r="L41" s="3" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="33"/>
         <v>Seed</v>
       </c>
       <c r="M41" s="3" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="33"/>
         <v>Seed</v>
       </c>
       <c r="N41" s="3" t="str">
-        <f t="shared" si="34"/>
-        <v>Seed</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="33"/>
+        <v>Seed</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" s="9"/>
       <c r="B42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C42" s="4">
         <v>45200</v>
       </c>
       <c r="D42" s="4">
-        <f t="shared" ref="D42:N42" si="35">C42</f>
+        <f t="shared" ref="D42:N42" si="34">C42</f>
         <v>45200</v>
       </c>
       <c r="E42" s="4">
-        <f t="shared" si="35"/>
+        <f t="shared" si="34"/>
         <v>45200</v>
       </c>
       <c r="F42" s="4">
-        <f t="shared" si="35"/>
+        <f t="shared" si="34"/>
         <v>45200</v>
       </c>
       <c r="G42" s="4">
-        <f t="shared" si="35"/>
+        <f t="shared" si="34"/>
         <v>45200</v>
       </c>
       <c r="H42" s="4">
-        <f t="shared" si="35"/>
+        <f t="shared" si="34"/>
         <v>45200</v>
       </c>
       <c r="I42" s="6">
         <v>45352</v>
       </c>
       <c r="J42" s="6">
-        <f t="shared" si="35"/>
+        <f t="shared" si="34"/>
         <v>45352</v>
       </c>
       <c r="K42" s="6">
-        <f t="shared" si="35"/>
+        <f t="shared" si="34"/>
         <v>45352</v>
       </c>
       <c r="L42" s="6">
-        <f t="shared" si="35"/>
+        <f t="shared" si="34"/>
         <v>45352</v>
       </c>
       <c r="M42" s="6">
-        <f t="shared" si="35"/>
+        <f t="shared" si="34"/>
         <v>45352</v>
       </c>
       <c r="N42" s="6">
-        <f t="shared" si="35"/>
+        <f t="shared" si="34"/>
         <v>45352</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43" s="9"/>
       <c r="B43" t="s">
+        <v>43</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C43" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="D43" s="3" t="str">
-        <f t="shared" ref="D43:N43" si="36">C43</f>
+        <f t="shared" ref="D43:N43" si="35">C43</f>
         <v>EarlyReproductive</v>
       </c>
       <c r="E43" s="3" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>EarlyReproductive</v>
       </c>
       <c r="F43" s="3" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>EarlyReproductive</v>
       </c>
       <c r="G43" s="3" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>EarlyReproductive</v>
       </c>
       <c r="H43" s="3" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>EarlyReproductive</v>
       </c>
       <c r="I43" s="3" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>EarlyReproductive</v>
       </c>
       <c r="J43" s="3" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>EarlyReproductive</v>
       </c>
       <c r="K43" s="3" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>EarlyReproductive</v>
       </c>
       <c r="L43" s="3" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>EarlyReproductive</v>
       </c>
       <c r="M43" s="3" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>EarlyReproductive</v>
       </c>
       <c r="N43" s="3" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>EarlyReproductive</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A44" s="9"/>
       <c r="B44" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C44" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D44" t="str">
-        <f t="shared" ref="D44:N44" si="37">C44</f>
+        <f t="shared" ref="D44:N44" si="36">C44</f>
         <v>None removed</v>
       </c>
       <c r="E44" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>None removed</v>
       </c>
       <c r="F44" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>None removed</v>
       </c>
       <c r="G44" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>None removed</v>
       </c>
       <c r="H44" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>None removed</v>
       </c>
       <c r="I44" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>None removed</v>
       </c>
       <c r="J44" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>None removed</v>
       </c>
       <c r="K44" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>None removed</v>
       </c>
       <c r="L44" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>None removed</v>
       </c>
       <c r="M44" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>None removed</v>
       </c>
       <c r="N44" t="str">
-        <f t="shared" si="37"/>
-        <v>None removed</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="36"/>
+        <v>None removed</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="10"/>
       <c r="B45" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D45" s="1" t="str">
-        <f t="shared" ref="D45:N45" si="38">C45</f>
+        <f t="shared" ref="D45:N45" si="37">C45</f>
         <v>Full (Plough)</v>
       </c>
       <c r="E45" s="1" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>Full (Plough)</v>
       </c>
       <c r="F45" s="1" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>Full (Plough)</v>
       </c>
       <c r="G45" s="1" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>Full (Plough)</v>
       </c>
       <c r="H45" s="1" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>Full (Plough)</v>
       </c>
       <c r="I45" s="1" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>Full (Plough)</v>
       </c>
       <c r="J45" s="1" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>Full (Plough)</v>
       </c>
       <c r="K45" s="1" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>Full (Plough)</v>
       </c>
       <c r="L45" s="1" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>Full (Plough)</v>
       </c>
       <c r="M45" s="1" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>Full (Plough)</v>
       </c>
       <c r="N45" s="1" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>Full (Plough)</v>
       </c>
     </row>

</xml_diff>